<commit_message>
EPBDS-9765 Add a validation transient fields for loaded classes.
--HG--
branch : EPBDS-9737
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-6830_external_datatypes_validation.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-6830_external_datatypes_validation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572E43AB-63F9-46E5-AD90-1872ACF5ED43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162C285A-814B-48F4-BDFB-0CD1DA2ABFE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1995" yWindow="1193" windowWidth="21600" windowHeight="11535" tabRatio="965" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" tabRatio="965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datatypes" sheetId="93" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
   <si>
     <t>String</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>org.openl.generated.epbds6830</t>
+  </si>
+  <si>
+    <t>xB~</t>
   </si>
 </sst>
 </file>
@@ -594,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.5"/>
@@ -694,7 +697,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1">
         <v>64</v>
@@ -846,7 +849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B3:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>